<commit_message>
Merge NguyenTrungNghia with NguyenTrungNghia-updated
</commit_message>
<xml_diff>
--- a/Lab01/NguyenTrungNghia/Flow of events.xlsx
+++ b/Lab01/NguyenTrungNghia/Flow of events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\JavaLab\CapstoneProject\NguyenTrungNghia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970AE095-B7CE-46D5-8BFC-C41733547D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC0D58F-F861-4C56-BBD9-28CE8484D1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4896" yWindow="1452" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,34 +46,34 @@
     <t>2a</t>
   </si>
   <si>
-    <t>View dock's information</t>
-  </si>
-  <si>
-    <t>login to view dock's information</t>
-  </si>
-  <si>
-    <t>check login information</t>
-  </si>
-  <si>
-    <t>choose a station to view information of bikes</t>
-  </si>
-  <si>
-    <t>show the view of dock's information</t>
-  </si>
-  <si>
-    <t>display detail information of all bikes at that dock</t>
-  </si>
-  <si>
     <t>View detail information of bikes at the dock</t>
   </si>
   <si>
-    <t>query for all bikes information related to that dock</t>
-  </si>
-  <si>
     <t>in case of database query failed, notify to the user, end of use case</t>
   </si>
   <si>
-    <t>in case of invalid login information, notify to the user, end of use case</t>
+    <t>View dock's information and avaiable bikes</t>
+  </si>
+  <si>
+    <t>click on a dock to see dock's detail information and avaiable bikes</t>
+  </si>
+  <si>
+    <t>update the number of avaiable bikes and e-bike's battery information</t>
+  </si>
+  <si>
+    <t>display the view of dock's information and avaiable bikes</t>
+  </si>
+  <si>
+    <t>in case of failed updating, notify to the user, end of use case</t>
+  </si>
+  <si>
+    <t>query for detail bike's information related to that bike</t>
+  </si>
+  <si>
+    <t>display detail bike's information</t>
+  </si>
+  <si>
+    <t>click on a bike in the list to see detail bike's information</t>
   </si>
 </sst>
 </file>
@@ -178,18 +178,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,8 +410,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -420,17 +420,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -451,8 +451,8 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>9</v>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -462,8 +462,8 @@
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>10</v>
+      <c r="C5" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -473,8 +473,8 @@
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>12</v>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -482,14 +482,14 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -507,39 +507,39 @@
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -557,8 +557,8 @@
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>11</v>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -579,28 +579,28 @@
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="15.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -618,8 +618,8 @@
       <c r="B24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>16</v>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -632,5 +632,6 @@
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>